<commit_message>
Actividad 6 (Regresión Lineal Simple y Múltiple) Completada
</commit_message>
<xml_diff>
--- a/Mejores-coeficientes.xlsx
+++ b/Mejores-coeficientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmanu\OneDrive\Escritorio\Inteligencia-de-Negocios\Regresion-Lineal-Simple-y-Multiple\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C60A5E67-DC5B-4547-9D63-AA3C7F8C455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6C544F-F015-433F-8610-E8DD5D8D8B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9F340A03-3596-4E79-A811-36D49174F8FF}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{9F340A03-3596-4E79-A811-36D49174F8FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -143,12 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -157,10 +154,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -504,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09DBA8B-1732-414C-9A5D-849CD757ACCF}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +535,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -551,14 +548,14 @@
         <v>9</v>
       </c>
       <c r="E2" s="1">
-        <v>0.1865</v>
+        <v>0.2026</v>
       </c>
       <c r="F2" s="1">
-        <v>3.4799999999999998E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -576,7 +573,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -594,7 +591,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
@@ -608,31 +605,31 @@
         <v>0.28349999999999997</v>
       </c>
       <c r="F5" s="1">
-        <v>8.0399999999999999E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0.1321</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -650,7 +647,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
@@ -668,7 +665,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>